<commit_message>
Move text from top and bottom to the side
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -232,10 +232,10 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.29"/>
   </cols>

</xml_diff>